<commit_message>
Update data to csv
</commit_message>
<xml_diff>
--- a/stats/dataset-cw.xlsx
+++ b/stats/dataset-cw.xlsx
@@ -377,7 +377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E803"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -419,7 +419,7 @@
         <v>1062</v>
       </c>
       <c r="E4" t="str">
-        <v>10.6</v>
+        <v>zzz</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Added stats in percentage
</commit_message>
<xml_diff>
--- a/stats/dataset-cw.xlsx
+++ b/stats/dataset-cw.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F244"/>
+  <dimension ref="A1:H244"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -404,6 +404,12 @@
       <c r="F4" t="str">
         <v>cpx</v>
       </c>
+      <c r="G4" t="str">
+        <v>bp_percent</v>
+      </c>
+      <c r="H4" t="str">
+        <v>cpx_percent</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" t="str">
@@ -421,6 +427,12 @@
       <c r="F5">
         <v>10.6</v>
       </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="str">
@@ -438,6 +450,12 @@
       <c r="F6">
         <v>11.1</v>
       </c>
+      <c r="G6">
+        <v>46.333333333333336</v>
+      </c>
+      <c r="H6">
+        <v>104.71698113207547</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" t="str">
@@ -455,6 +473,12 @@
       <c r="F7">
         <v>15</v>
       </c>
+      <c r="G7">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="H7">
+        <v>141.50943396226415</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" t="str">
@@ -472,6 +496,12 @@
       <c r="F8">
         <v>7.7</v>
       </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="str">
@@ -489,6 +519,12 @@
       <c r="F9">
         <v>8.9</v>
       </c>
+      <c r="G9">
+        <v>6.219151036525172</v>
+      </c>
+      <c r="H9">
+        <v>115.58441558441558</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" t="str">
@@ -506,6 +542,12 @@
       <c r="F10">
         <v>7.7</v>
       </c>
+      <c r="G10">
+        <v>5.923000987166831</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" t="str">
@@ -523,6 +565,12 @@
       <c r="F11">
         <v>7.5</v>
       </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="str">
@@ -540,6 +588,12 @@
       <c r="F12">
         <v>11.8</v>
       </c>
+      <c r="G12">
+        <v>63.116883116883116</v>
+      </c>
+      <c r="H12">
+        <v>157.33333333333334</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" t="str">
@@ -557,6 +611,12 @@
       <c r="F13">
         <v>6.8</v>
       </c>
+      <c r="G13">
+        <v>12.987012987012987</v>
+      </c>
+      <c r="H13">
+        <v>90.66666666666667</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" t="str">
@@ -574,6 +634,12 @@
       <c r="F14">
         <v>2.2</v>
       </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="str">
@@ -591,6 +657,12 @@
       <c r="F15">
         <v>11.7</v>
       </c>
+      <c r="G15">
+        <v>24.673439767779392</v>
+      </c>
+      <c r="H15">
+        <v>531.8181818181818</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" t="str">
@@ -608,6 +680,12 @@
       <c r="F16">
         <v>11.1</v>
       </c>
+      <c r="G16">
+        <v>7.547169811320755</v>
+      </c>
+      <c r="H16">
+        <v>504.5454545454545</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" t="str">
@@ -625,6 +703,12 @@
       <c r="F17">
         <v>12.7</v>
       </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="str">
@@ -642,6 +726,12 @@
       <c r="F18">
         <v>9.5</v>
       </c>
+      <c r="G18">
+        <v>21.035598705501616</v>
+      </c>
+      <c r="H18">
+        <v>74.80314960629921</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" t="str">
@@ -659,6 +749,12 @@
       <c r="F19">
         <v>13.6</v>
       </c>
+      <c r="G19">
+        <v>7.44336569579288</v>
+      </c>
+      <c r="H19">
+        <v>107.08661417322836</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" t="str">
@@ -676,6 +772,12 @@
       <c r="F20">
         <v>12</v>
       </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="str">
@@ -693,6 +795,12 @@
       <c r="F21">
         <v>5.6</v>
       </c>
+      <c r="G21">
+        <v>21.073170731707318</v>
+      </c>
+      <c r="H21">
+        <v>46.666666666666664</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" t="str">
@@ -710,6 +818,12 @@
       <c r="F22">
         <v>12.6</v>
       </c>
+      <c r="G22">
+        <v>18.634146341463413</v>
+      </c>
+      <c r="H22">
+        <v>105</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" t="str">
@@ -727,6 +841,12 @@
       <c r="F23">
         <v>13.1</v>
       </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" t="str">
@@ -744,6 +864,12 @@
       <c r="F24">
         <v>11.6</v>
       </c>
+      <c r="G24">
+        <v>17.4573055028463</v>
+      </c>
+      <c r="H24">
+        <v>88.54961832061069</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" t="str">
@@ -761,6 +887,12 @@
       <c r="F25">
         <v>10.3</v>
       </c>
+      <c r="G25">
+        <v>12.903225806451612</v>
+      </c>
+      <c r="H25">
+        <v>78.62595419847328</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" t="str">
@@ -778,6 +910,12 @@
       <c r="F26">
         <v>7.9</v>
       </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" t="str">
@@ -795,6 +933,12 @@
       <c r="F27">
         <v>5.4</v>
       </c>
+      <c r="G27">
+        <v>99.86910994764398</v>
+      </c>
+      <c r="H27">
+        <v>68.35443037974683</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" t="str">
@@ -812,6 +956,12 @@
       <c r="F28">
         <v>6.5</v>
       </c>
+      <c r="G28">
+        <v>44.24083769633508</v>
+      </c>
+      <c r="H28">
+        <v>82.27848101265822</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" t="str">
@@ -829,6 +979,12 @@
       <c r="F29">
         <v>6.5</v>
       </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>100</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" t="str">
@@ -846,6 +1002,12 @@
       <c r="F30">
         <v>5.8</v>
       </c>
+      <c r="G30">
+        <v>53.43434343434343</v>
+      </c>
+      <c r="H30">
+        <v>89.23076923076923</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" t="str">
@@ -863,6 +1025,12 @@
       <c r="F31">
         <v>7</v>
       </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>107.6923076923077</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" t="str">
@@ -880,6 +1048,12 @@
       <c r="F32">
         <v>5.2</v>
       </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" t="str">
@@ -897,6 +1071,12 @@
       <c r="F33">
         <v>6</v>
       </c>
+      <c r="G33">
+        <v>23.674911660777386</v>
+      </c>
+      <c r="H33">
+        <v>115.38461538461539</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" t="str">
@@ -914,6 +1094,12 @@
       <c r="F34">
         <v>5.5</v>
       </c>
+      <c r="G34">
+        <v>21.554770318021202</v>
+      </c>
+      <c r="H34">
+        <v>105.76923076923076</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" t="str">
@@ -931,6 +1117,12 @@
       <c r="F35">
         <v>11.8</v>
       </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>100</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" t="str">
@@ -948,6 +1140,12 @@
       <c r="F36">
         <v>12.8</v>
       </c>
+      <c r="G36">
+        <v>30.192307692307693</v>
+      </c>
+      <c r="H36">
+        <v>108.47457627118644</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" t="str">
@@ -965,6 +1163,12 @@
       <c r="F37">
         <v>11.8</v>
       </c>
+      <c r="G37">
+        <v>14.807692307692308</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" t="str">
@@ -982,6 +1186,12 @@
       <c r="F38">
         <v>13</v>
       </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" t="str">
@@ -999,6 +1209,12 @@
       <c r="F39">
         <v>11.3</v>
       </c>
+      <c r="G39">
+        <v>20.88724584103512</v>
+      </c>
+      <c r="H39">
+        <v>86.92307692307692</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" t="str">
@@ -1016,6 +1232,12 @@
       <c r="F40">
         <v>12.7</v>
       </c>
+      <c r="G40">
+        <v>12.199630314232902</v>
+      </c>
+      <c r="H40">
+        <v>97.6923076923077</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" t="str">
@@ -1033,6 +1255,12 @@
       <c r="F41">
         <v>10.6</v>
       </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>100</v>
+      </c>
     </row>
     <row r="42">
       <c r="B42" t="str">
@@ -1050,6 +1278,12 @@
       <c r="F42">
         <v>18.3</v>
       </c>
+      <c r="G42">
+        <v>23.343373493975903</v>
+      </c>
+      <c r="H42">
+        <v>172.64150943396228</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" t="str">
@@ -1067,6 +1301,12 @@
       <c r="F43">
         <v>21.7</v>
       </c>
+      <c r="G43">
+        <v>12.349397590361447</v>
+      </c>
+      <c r="H43">
+        <v>204.7169811320755</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" t="str">
@@ -1084,6 +1324,12 @@
       <c r="F44">
         <v>7.4</v>
       </c>
+      <c r="G44">
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>100</v>
+      </c>
     </row>
     <row r="45">
       <c r="B45" t="str">
@@ -1101,6 +1347,12 @@
       <c r="F45">
         <v>6.9</v>
       </c>
+      <c r="G45">
+        <v>54.67032967032967</v>
+      </c>
+      <c r="H45">
+        <v>93.24324324324324</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" t="str">
@@ -1118,6 +1370,12 @@
       <c r="F46">
         <v>6.1</v>
       </c>
+      <c r="G46">
+        <v>33.79120879120879</v>
+      </c>
+      <c r="H46">
+        <v>82.43243243243244</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" t="str">
@@ -1135,6 +1393,12 @@
       <c r="F47">
         <v>5.7</v>
       </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+      <c r="H47">
+        <v>100</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" t="str">
@@ -1152,6 +1416,12 @@
       <c r="F48">
         <v>5.2</v>
       </c>
+      <c r="G48">
+        <v>9.877488514548238</v>
+      </c>
+      <c r="H48">
+        <v>91.22807017543859</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" t="str">
@@ -1169,6 +1439,12 @@
       <c r="F49">
         <v>7.6</v>
       </c>
+      <c r="G49">
+        <v>5.359877488514548</v>
+      </c>
+      <c r="H49">
+        <v>133.33333333333334</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" t="str">
@@ -1186,6 +1462,12 @@
       <c r="F50">
         <v>7.4</v>
       </c>
+      <c r="G50">
+        <v>100</v>
+      </c>
+      <c r="H50">
+        <v>100</v>
+      </c>
     </row>
     <row r="51">
       <c r="B51" t="str">
@@ -1203,6 +1485,12 @@
       <c r="F51">
         <v>11.1</v>
       </c>
+      <c r="G51">
+        <v>24.84472049689441</v>
+      </c>
+      <c r="H51">
+        <v>150</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" t="str">
@@ -1220,6 +1508,12 @@
       <c r="F52">
         <v>8.4</v>
       </c>
+      <c r="G52">
+        <v>15.320910973084887</v>
+      </c>
+      <c r="H52">
+        <v>113.5135135135135</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" t="str">
@@ -1237,6 +1531,12 @@
       <c r="F53">
         <v>11.8</v>
       </c>
+      <c r="G53">
+        <v>100</v>
+      </c>
+      <c r="H53">
+        <v>100</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" t="str">
@@ -1254,6 +1554,12 @@
       <c r="F54">
         <v>9.6</v>
       </c>
+      <c r="G54">
+        <v>9.491978609625669</v>
+      </c>
+      <c r="H54">
+        <v>81.35593220338983</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" t="str">
@@ -1271,6 +1577,12 @@
       <c r="F55">
         <v>13.9</v>
       </c>
+      <c r="G55">
+        <v>8.02139037433155</v>
+      </c>
+      <c r="H55">
+        <v>117.79661016949152</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" t="str">
@@ -1288,6 +1600,12 @@
       <c r="F56">
         <v>18.1</v>
       </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>100</v>
+      </c>
     </row>
     <row r="57">
       <c r="B57" t="str">
@@ -1305,6 +1623,12 @@
       <c r="F57">
         <v>15.3</v>
       </c>
+      <c r="G57">
+        <v>23.716381418092908</v>
+      </c>
+      <c r="H57">
+        <v>84.53038674033148</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" t="str">
@@ -1322,6 +1646,12 @@
       <c r="F58">
         <v>14.2</v>
       </c>
+      <c r="G58">
+        <v>19.070904645476773</v>
+      </c>
+      <c r="H58">
+        <v>78.45303867403314</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" t="str">
@@ -1339,6 +1669,12 @@
       <c r="F59">
         <v>8.7</v>
       </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+      <c r="H59">
+        <v>100</v>
+      </c>
     </row>
     <row r="60">
       <c r="B60" t="str">
@@ -1356,6 +1692,12 @@
       <c r="F60">
         <v>8.3</v>
       </c>
+      <c r="G60">
+        <v>51.785714285714285</v>
+      </c>
+      <c r="H60">
+        <v>95.40229885057474</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" t="str">
@@ -1373,6 +1715,12 @@
       <c r="F61">
         <v>16.5</v>
       </c>
+      <c r="G61">
+        <v>9.226190476190476</v>
+      </c>
+      <c r="H61">
+        <v>189.6551724137931</v>
+      </c>
     </row>
     <row r="62">
       <c r="B62" t="str">
@@ -1390,6 +1738,12 @@
       <c r="F62">
         <v>11.8</v>
       </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="H62">
+        <v>100</v>
+      </c>
     </row>
     <row r="63">
       <c r="B63" t="str">
@@ -1407,6 +1761,12 @@
       <c r="F63">
         <v>5</v>
       </c>
+      <c r="G63">
+        <v>21.409921671018278</v>
+      </c>
+      <c r="H63">
+        <v>42.3728813559322</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" t="str">
@@ -1424,6 +1784,12 @@
       <c r="F64">
         <v>12.5</v>
       </c>
+      <c r="G64">
+        <v>14.099216710182768</v>
+      </c>
+      <c r="H64">
+        <v>105.9322033898305</v>
+      </c>
     </row>
     <row r="65">
       <c r="B65" t="str">
@@ -1441,6 +1807,12 @@
       <c r="F65">
         <v>6</v>
       </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+      <c r="H65">
+        <v>100</v>
+      </c>
     </row>
     <row r="66">
       <c r="B66" t="str">
@@ -1458,6 +1830,12 @@
       <c r="F66">
         <v>9.4</v>
       </c>
+      <c r="G66">
+        <v>15.954773869346734</v>
+      </c>
+      <c r="H66">
+        <v>156.66666666666666</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" t="str">
@@ -1475,6 +1853,12 @@
       <c r="F67">
         <v>5</v>
       </c>
+      <c r="G67">
+        <v>11.4321608040201</v>
+      </c>
+      <c r="H67">
+        <v>83.33333333333333</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" t="str">
@@ -1492,6 +1876,12 @@
       <c r="F68">
         <v>4.8</v>
       </c>
+      <c r="G68">
+        <v>100</v>
+      </c>
+      <c r="H68">
+        <v>100</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" t="str">
@@ -1509,6 +1899,12 @@
       <c r="F69">
         <v>6.1</v>
       </c>
+      <c r="G69">
+        <v>7.387387387387387</v>
+      </c>
+      <c r="H69">
+        <v>127.08333333333334</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" t="str">
@@ -1526,6 +1922,12 @@
       <c r="F70">
         <v>0</v>
       </c>
+      <c r="G70">
+        <v>7.207207207207207</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" t="str">
@@ -1543,6 +1945,12 @@
       <c r="F71">
         <v>8.1</v>
       </c>
+      <c r="G71">
+        <v>100</v>
+      </c>
+      <c r="H71">
+        <v>100</v>
+      </c>
     </row>
     <row r="72">
       <c r="B72" t="str">
@@ -1560,6 +1968,12 @@
       <c r="F72">
         <v>10.7</v>
       </c>
+      <c r="G72">
+        <v>31.645569620253166</v>
+      </c>
+      <c r="H72">
+        <v>132.09876543209876</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" t="str">
@@ -1577,6 +1991,12 @@
       <c r="F73">
         <v>8.1</v>
       </c>
+      <c r="G73">
+        <v>23.417721518987342</v>
+      </c>
+      <c r="H73">
+        <v>100</v>
+      </c>
     </row>
     <row r="74">
       <c r="B74" t="str">
@@ -1594,6 +2014,12 @@
       <c r="F74">
         <v>7.5</v>
       </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+      <c r="H74">
+        <v>100</v>
+      </c>
     </row>
     <row r="75">
       <c r="B75" t="str">
@@ -1611,6 +2037,12 @@
       <c r="F75">
         <v>5.6</v>
       </c>
+      <c r="G75">
+        <v>67.37588652482269</v>
+      </c>
+      <c r="H75">
+        <v>74.66666666666667</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" t="str">
@@ -1628,6 +2060,12 @@
       <c r="F76">
         <v>6.1</v>
       </c>
+      <c r="G76">
+        <v>10.99290780141844</v>
+      </c>
+      <c r="H76">
+        <v>81.33333333333333</v>
+      </c>
     </row>
     <row r="77">
       <c r="B77" t="str">
@@ -1645,6 +2083,12 @@
       <c r="F77">
         <v>6.4</v>
       </c>
+      <c r="G77">
+        <v>100</v>
+      </c>
+      <c r="H77">
+        <v>100</v>
+      </c>
     </row>
     <row r="78">
       <c r="B78" t="str">
@@ -1662,6 +2106,12 @@
       <c r="F78">
         <v>7.9</v>
       </c>
+      <c r="G78">
+        <v>28.29787234042553</v>
+      </c>
+      <c r="H78">
+        <v>123.4375</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" t="str">
@@ -1679,6 +2129,12 @@
       <c r="F79">
         <v>3.9</v>
       </c>
+      <c r="G79">
+        <v>18.72340425531915</v>
+      </c>
+      <c r="H79">
+        <v>60.9375</v>
+      </c>
     </row>
     <row r="80">
       <c r="B80" t="str">
@@ -1696,6 +2152,12 @@
       <c r="F80">
         <v>3.2</v>
       </c>
+      <c r="G80">
+        <v>100</v>
+      </c>
+      <c r="H80">
+        <v>100</v>
+      </c>
     </row>
     <row r="81">
       <c r="B81" t="str">
@@ -1713,6 +2175,12 @@
       <c r="F81">
         <v>3.9</v>
       </c>
+      <c r="G81">
+        <v>25.358490566037737</v>
+      </c>
+      <c r="H81">
+        <v>121.875</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" t="str">
@@ -1730,6 +2198,12 @@
       <c r="F82">
         <v>4.1</v>
       </c>
+      <c r="G82">
+        <v>14.11320754716981</v>
+      </c>
+      <c r="H82">
+        <v>128.12499999999997</v>
+      </c>
     </row>
     <row r="83">
       <c r="B83" t="str">
@@ -1747,6 +2221,12 @@
       <c r="F83">
         <v>8.4</v>
       </c>
+      <c r="G83">
+        <v>100</v>
+      </c>
+      <c r="H83">
+        <v>100</v>
+      </c>
     </row>
     <row r="84">
       <c r="B84" t="str">
@@ -1764,6 +2244,12 @@
       <c r="F84">
         <v>7.2</v>
       </c>
+      <c r="G84">
+        <v>9.956709956709958</v>
+      </c>
+      <c r="H84">
+        <v>85.71428571428571</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" t="str">
@@ -1781,6 +2267,12 @@
       <c r="F85">
         <v>8.5</v>
       </c>
+      <c r="G85">
+        <v>7.575757575757576</v>
+      </c>
+      <c r="H85">
+        <v>101.19047619047619</v>
+      </c>
     </row>
     <row r="86">
       <c r="B86" t="str">
@@ -1798,6 +2290,12 @@
       <c r="F86">
         <v>11.3</v>
       </c>
+      <c r="G86">
+        <v>100</v>
+      </c>
+      <c r="H86">
+        <v>100</v>
+      </c>
     </row>
     <row r="87">
       <c r="B87" t="str">
@@ -1815,6 +2313,12 @@
       <c r="F87">
         <v>12.6</v>
       </c>
+      <c r="G87">
+        <v>19.167904903417533</v>
+      </c>
+      <c r="H87">
+        <v>111.50442477876105</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" t="str">
@@ -1832,6 +2336,12 @@
       <c r="F88">
         <v>12.7</v>
       </c>
+      <c r="G88">
+        <v>10.846953937592868</v>
+      </c>
+      <c r="H88">
+        <v>112.38938053097344</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" t="str">
@@ -1849,6 +2359,12 @@
       <c r="F89">
         <v>7.7</v>
       </c>
+      <c r="G89">
+        <v>100</v>
+      </c>
+      <c r="H89">
+        <v>100</v>
+      </c>
     </row>
     <row r="90">
       <c r="B90" t="str">
@@ -1866,6 +2382,12 @@
       <c r="F90">
         <v>7.6</v>
       </c>
+      <c r="G90">
+        <v>70.33248081841433</v>
+      </c>
+      <c r="H90">
+        <v>98.7012987012987</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" t="str">
@@ -1883,6 +2405,12 @@
       <c r="F91">
         <v>8</v>
       </c>
+      <c r="G91">
+        <v>34.271099744245525</v>
+      </c>
+      <c r="H91">
+        <v>103.8961038961039</v>
+      </c>
     </row>
     <row r="92">
       <c r="B92" t="str">
@@ -1900,6 +2428,12 @@
       <c r="F92">
         <v>10.2</v>
       </c>
+      <c r="G92">
+        <v>100</v>
+      </c>
+      <c r="H92">
+        <v>100</v>
+      </c>
     </row>
     <row r="93">
       <c r="B93" t="str">
@@ -1917,6 +2451,12 @@
       <c r="F93">
         <v>12</v>
       </c>
+      <c r="G93">
+        <v>26.34508348794063</v>
+      </c>
+      <c r="H93">
+        <v>117.64705882352942</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" t="str">
@@ -1934,6 +2474,12 @@
       <c r="F94">
         <v>7.7</v>
       </c>
+      <c r="G94">
+        <v>12.059369202226344</v>
+      </c>
+      <c r="H94">
+        <v>75.49019607843138</v>
+      </c>
     </row>
     <row r="95">
       <c r="B95" t="str">
@@ -1951,6 +2497,12 @@
       <c r="F95">
         <v>0</v>
       </c>
+      <c r="G95">
+        <v>100</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="B96" t="str">
@@ -1968,6 +2520,12 @@
       <c r="F96">
         <v>0</v>
       </c>
+      <c r="G96">
+        <v>21.566731141199227</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" t="str">
@@ -1985,6 +2543,12 @@
       <c r="F97">
         <v>0</v>
       </c>
+      <c r="G97">
+        <v>11.218568665377177</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="B98" t="str">
@@ -2002,6 +2566,12 @@
       <c r="F98">
         <v>5.7</v>
       </c>
+      <c r="G98">
+        <v>100</v>
+      </c>
+      <c r="H98">
+        <v>100</v>
+      </c>
     </row>
     <row r="99">
       <c r="B99" t="str">
@@ -2019,6 +2589,12 @@
       <c r="F99">
         <v>6.7</v>
       </c>
+      <c r="G99">
+        <v>53.099173553719005</v>
+      </c>
+      <c r="H99">
+        <v>117.54385964912281</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" t="str">
@@ -2036,6 +2612,12 @@
       <c r="F100">
         <v>6.4</v>
       </c>
+      <c r="G100">
+        <v>11.363636363636363</v>
+      </c>
+      <c r="H100">
+        <v>112.28070175438596</v>
+      </c>
     </row>
     <row r="101">
       <c r="B101" t="str">
@@ -2053,6 +2635,12 @@
       <c r="F101">
         <v>4.4</v>
       </c>
+      <c r="G101">
+        <v>100</v>
+      </c>
+      <c r="H101">
+        <v>100</v>
+      </c>
     </row>
     <row r="102">
       <c r="B102" t="str">
@@ -2070,6 +2658,12 @@
       <c r="F102">
         <v>5.3</v>
       </c>
+      <c r="G102">
+        <v>63.16568047337278</v>
+      </c>
+      <c r="H102">
+        <v>120.45454545454544</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" t="str">
@@ -2087,6 +2681,12 @@
       <c r="F103">
         <v>6.3</v>
       </c>
+      <c r="G103">
+        <v>23.668639053254438</v>
+      </c>
+      <c r="H103">
+        <v>143.18181818181816</v>
+      </c>
     </row>
     <row r="104">
       <c r="B104" t="str">
@@ -2104,6 +2704,12 @@
       <c r="F104">
         <v>4.7</v>
       </c>
+      <c r="G104">
+        <v>100</v>
+      </c>
+      <c r="H104">
+        <v>100</v>
+      </c>
     </row>
     <row r="105">
       <c r="B105" t="str">
@@ -2121,6 +2727,12 @@
       <c r="F105">
         <v>3.3</v>
       </c>
+      <c r="G105">
+        <v>81.26361655773421</v>
+      </c>
+      <c r="H105">
+        <v>70.2127659574468</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" t="str">
@@ -2138,6 +2750,12 @@
       <c r="F106">
         <v>10.6</v>
       </c>
+      <c r="G106">
+        <v>35.947712418300654</v>
+      </c>
+      <c r="H106">
+        <v>225.531914893617</v>
+      </c>
     </row>
     <row r="107">
       <c r="B107" t="str">
@@ -2155,6 +2773,12 @@
       <c r="F107">
         <v>5.9</v>
       </c>
+      <c r="G107">
+        <v>100</v>
+      </c>
+      <c r="H107">
+        <v>100</v>
+      </c>
     </row>
     <row r="108">
       <c r="B108" t="str">
@@ -2172,6 +2796,12 @@
       <c r="F108">
         <v>10.2</v>
       </c>
+      <c r="G108">
+        <v>22.374429223744293</v>
+      </c>
+      <c r="H108">
+        <v>172.88135593220335</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" t="str">
@@ -2189,6 +2819,12 @@
       <c r="F109">
         <v>4</v>
       </c>
+      <c r="G109">
+        <v>21.765601217656013</v>
+      </c>
+      <c r="H109">
+        <v>67.79661016949152</v>
+      </c>
     </row>
     <row r="110">
       <c r="B110" t="str">
@@ -2206,6 +2842,12 @@
       <c r="F110">
         <v>5.3</v>
       </c>
+      <c r="G110">
+        <v>100</v>
+      </c>
+      <c r="H110">
+        <v>100</v>
+      </c>
     </row>
     <row r="111">
       <c r="B111" t="str">
@@ -2223,6 +2865,12 @@
       <c r="F111">
         <v>6.1</v>
       </c>
+      <c r="G111">
+        <v>34.28165007112376</v>
+      </c>
+      <c r="H111">
+        <v>115.09433962264151</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" t="str">
@@ -2240,6 +2888,12 @@
       <c r="F112">
         <v>9.3</v>
       </c>
+      <c r="G112">
+        <v>10.81081081081081</v>
+      </c>
+      <c r="H112">
+        <v>175.47169811320757</v>
+      </c>
     </row>
     <row r="113">
       <c r="B113" t="str">
@@ -2257,6 +2911,12 @@
       <c r="F113">
         <v>6.8</v>
       </c>
+      <c r="G113">
+        <v>100</v>
+      </c>
+      <c r="H113">
+        <v>100</v>
+      </c>
     </row>
     <row r="114">
       <c r="B114" t="str">
@@ -2274,6 +2934,12 @@
       <c r="F114">
         <v>4.9</v>
       </c>
+      <c r="G114">
+        <v>28.17824377457405</v>
+      </c>
+      <c r="H114">
+        <v>72.05882352941177</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" t="str">
@@ -2291,6 +2957,12 @@
       <c r="F115">
         <v>4.9</v>
       </c>
+      <c r="G115">
+        <v>17.03800786369594</v>
+      </c>
+      <c r="H115">
+        <v>72.05882352941177</v>
+      </c>
     </row>
     <row r="116">
       <c r="B116" t="str">
@@ -2308,6 +2980,12 @@
       <c r="F116">
         <v>5</v>
       </c>
+      <c r="G116">
+        <v>100</v>
+      </c>
+      <c r="H116">
+        <v>100</v>
+      </c>
     </row>
     <row r="117">
       <c r="B117" t="str">
@@ -2325,6 +3003,12 @@
       <c r="F117">
         <v>4.9</v>
       </c>
+      <c r="G117">
+        <v>96.63608562691131</v>
+      </c>
+      <c r="H117">
+        <v>98.00000000000001</v>
+      </c>
     </row>
     <row r="118">
       <c r="B118" t="str">
@@ -2342,6 +3026,12 @@
       <c r="F118">
         <v>9.3</v>
       </c>
+      <c r="G118">
+        <v>14.37308868501529</v>
+      </c>
+      <c r="H118">
+        <v>186.00000000000003</v>
+      </c>
     </row>
     <row r="119">
       <c r="B119" t="str">
@@ -2359,6 +3049,12 @@
       <c r="F119">
         <v>5.8</v>
       </c>
+      <c r="G119">
+        <v>100</v>
+      </c>
+      <c r="H119">
+        <v>100</v>
+      </c>
     </row>
     <row r="120">
       <c r="B120" t="str">
@@ -2376,6 +3072,12 @@
       <c r="F120">
         <v>7</v>
       </c>
+      <c r="G120">
+        <v>6.142857142857143</v>
+      </c>
+      <c r="H120">
+        <v>120.6896551724138</v>
+      </c>
     </row>
     <row r="121">
       <c r="B121" t="str">
@@ -2393,6 +3095,12 @@
       <c r="F121">
         <v>4.1</v>
       </c>
+      <c r="G121">
+        <v>5.714285714285714</v>
+      </c>
+      <c r="H121">
+        <v>70.68965517241378</v>
+      </c>
     </row>
     <row r="122">
       <c r="B122" t="str">
@@ -2410,6 +3118,12 @@
       <c r="F122">
         <v>4.4</v>
       </c>
+      <c r="G122">
+        <v>100</v>
+      </c>
+      <c r="H122">
+        <v>100</v>
+      </c>
     </row>
     <row r="123">
       <c r="B123" t="str">
@@ -2427,6 +3141,12 @@
       <c r="F123">
         <v>5.7</v>
       </c>
+      <c r="G123">
+        <v>26.013513513513512</v>
+      </c>
+      <c r="H123">
+        <v>129.54545454545453</v>
+      </c>
     </row>
     <row r="124">
       <c r="B124" t="str">
@@ -2444,6 +3164,12 @@
       <c r="F124">
         <v>9.9</v>
       </c>
+      <c r="G124">
+        <v>5.236486486486487</v>
+      </c>
+      <c r="H124">
+        <v>224.99999999999997</v>
+      </c>
     </row>
     <row r="125">
       <c r="B125" t="str">
@@ -2461,6 +3187,12 @@
       <c r="F125">
         <v>10.5</v>
       </c>
+      <c r="G125">
+        <v>100</v>
+      </c>
+      <c r="H125">
+        <v>100</v>
+      </c>
     </row>
     <row r="126">
       <c r="B126" t="str">
@@ -2478,6 +3210,12 @@
       <c r="F126">
         <v>11.1</v>
       </c>
+      <c r="G126">
+        <v>30.434782608695652</v>
+      </c>
+      <c r="H126">
+        <v>105.71428571428571</v>
+      </c>
     </row>
     <row r="127">
       <c r="B127" t="str">
@@ -2495,6 +3233,12 @@
       <c r="F127">
         <v>12.3</v>
       </c>
+      <c r="G127">
+        <v>14.130434782608695</v>
+      </c>
+      <c r="H127">
+        <v>117.14285714285714</v>
+      </c>
     </row>
     <row r="128">
       <c r="B128" t="str">
@@ -2512,6 +3256,12 @@
       <c r="F128">
         <v>5.5</v>
       </c>
+      <c r="G128">
+        <v>100</v>
+      </c>
+      <c r="H128">
+        <v>100</v>
+      </c>
     </row>
     <row r="129">
       <c r="B129" t="str">
@@ -2529,6 +3279,12 @@
       <c r="F129">
         <v>8.4</v>
       </c>
+      <c r="G129">
+        <v>21.3953488372093</v>
+      </c>
+      <c r="H129">
+        <v>152.72727272727272</v>
+      </c>
     </row>
     <row r="130">
       <c r="B130" t="str">
@@ -2546,6 +3302,12 @@
       <c r="F130">
         <v>10</v>
       </c>
+      <c r="G130">
+        <v>8.13953488372093</v>
+      </c>
+      <c r="H130">
+        <v>181.8181818181818</v>
+      </c>
     </row>
     <row r="131">
       <c r="B131" t="str">
@@ -2563,6 +3325,12 @@
       <c r="F131">
         <v>13.3</v>
       </c>
+      <c r="G131">
+        <v>100</v>
+      </c>
+      <c r="H131">
+        <v>100</v>
+      </c>
     </row>
     <row r="132">
       <c r="B132" t="str">
@@ -2580,6 +3348,12 @@
       <c r="F132">
         <v>14</v>
       </c>
+      <c r="G132">
+        <v>47.08029197080292</v>
+      </c>
+      <c r="H132">
+        <v>105.26315789473684</v>
+      </c>
     </row>
     <row r="133">
       <c r="B133" t="str">
@@ -2597,6 +3371,12 @@
       <c r="F133">
         <v>11.8</v>
       </c>
+      <c r="G133">
+        <v>15.693430656934307</v>
+      </c>
+      <c r="H133">
+        <v>88.7218045112782</v>
+      </c>
     </row>
     <row r="134">
       <c r="B134" t="str">
@@ -2614,6 +3394,12 @@
       <c r="F134">
         <v>10.2</v>
       </c>
+      <c r="G134">
+        <v>100</v>
+      </c>
+      <c r="H134">
+        <v>100</v>
+      </c>
     </row>
     <row r="135">
       <c r="B135" t="str">
@@ -2631,6 +3417,12 @@
       <c r="F135">
         <v>13</v>
       </c>
+      <c r="G135">
+        <v>55.89041095890411</v>
+      </c>
+      <c r="H135">
+        <v>127.45098039215686</v>
+      </c>
     </row>
     <row r="136">
       <c r="B136" t="str">
@@ -2648,6 +3440,12 @@
       <c r="F136">
         <v>7.8</v>
       </c>
+      <c r="G136">
+        <v>27.945205479452056</v>
+      </c>
+      <c r="H136">
+        <v>76.47058823529412</v>
+      </c>
     </row>
     <row r="137">
       <c r="B137" t="str">
@@ -2665,6 +3463,12 @@
       <c r="F137">
         <v>15.3</v>
       </c>
+      <c r="G137">
+        <v>100</v>
+      </c>
+      <c r="H137">
+        <v>100</v>
+      </c>
     </row>
     <row r="138">
       <c r="B138" t="str">
@@ -2682,6 +3486,12 @@
       <c r="F138">
         <v>12.3</v>
       </c>
+      <c r="G138">
+        <v>21.153846153846153</v>
+      </c>
+      <c r="H138">
+        <v>80.3921568627451</v>
+      </c>
     </row>
     <row r="139">
       <c r="B139" t="str">
@@ -2699,6 +3509,12 @@
       <c r="F139">
         <v>19.9</v>
       </c>
+      <c r="G139">
+        <v>17.032967032967033</v>
+      </c>
+      <c r="H139">
+        <v>130.06535947712416</v>
+      </c>
     </row>
     <row r="140">
       <c r="B140" t="str">
@@ -2716,6 +3532,12 @@
       <c r="F140">
         <v>6.8</v>
       </c>
+      <c r="G140">
+        <v>100</v>
+      </c>
+      <c r="H140">
+        <v>100</v>
+      </c>
     </row>
     <row r="141">
       <c r="B141" t="str">
@@ -2733,6 +3555,12 @@
       <c r="F141">
         <v>11.9</v>
       </c>
+      <c r="G141">
+        <v>57.429718875502004</v>
+      </c>
+      <c r="H141">
+        <v>175</v>
+      </c>
     </row>
     <row r="142">
       <c r="B142" t="str">
@@ -2750,6 +3578,12 @@
       <c r="F142">
         <v>12.4</v>
       </c>
+      <c r="G142">
+        <v>22.89156626506024</v>
+      </c>
+      <c r="H142">
+        <v>182.35294117647058</v>
+      </c>
     </row>
     <row r="143">
       <c r="B143" t="str">
@@ -2767,6 +3601,12 @@
       <c r="F143">
         <v>10.8</v>
       </c>
+      <c r="G143">
+        <v>100</v>
+      </c>
+      <c r="H143">
+        <v>100</v>
+      </c>
     </row>
     <row r="144">
       <c r="B144" t="str">
@@ -2784,6 +3624,12 @@
       <c r="F144">
         <v>18.1</v>
       </c>
+      <c r="G144">
+        <v>15.15748031496063</v>
+      </c>
+      <c r="H144">
+        <v>167.5925925925926</v>
+      </c>
     </row>
     <row r="145">
       <c r="B145" t="str">
@@ -2801,6 +3647,12 @@
       <c r="F145">
         <v>11.8</v>
       </c>
+      <c r="G145">
+        <v>5.905511811023622</v>
+      </c>
+      <c r="H145">
+        <v>109.25925925925925</v>
+      </c>
     </row>
     <row r="146">
       <c r="B146" t="str">
@@ -2818,6 +3670,12 @@
       <c r="F146">
         <v>8.8</v>
       </c>
+      <c r="G146">
+        <v>100</v>
+      </c>
+      <c r="H146">
+        <v>100</v>
+      </c>
     </row>
     <row r="147">
       <c r="B147" t="str">
@@ -2835,6 +3693,12 @@
       <c r="F147">
         <v>13</v>
       </c>
+      <c r="G147">
+        <v>47.44897959183673</v>
+      </c>
+      <c r="H147">
+        <v>147.72727272727272</v>
+      </c>
     </row>
     <row r="148">
       <c r="B148" t="str">
@@ -2852,6 +3716,12 @@
       <c r="F148">
         <v>19.3</v>
       </c>
+      <c r="G148">
+        <v>22.448979591836736</v>
+      </c>
+      <c r="H148">
+        <v>219.3181818181818</v>
+      </c>
     </row>
     <row r="149">
       <c r="B149" t="str">
@@ -2869,6 +3739,12 @@
       <c r="F149">
         <v>9.2</v>
       </c>
+      <c r="G149">
+        <v>100</v>
+      </c>
+      <c r="H149">
+        <v>100</v>
+      </c>
     </row>
     <row r="150">
       <c r="B150" t="str">
@@ -2886,6 +3762,12 @@
       <c r="F150">
         <v>9</v>
       </c>
+      <c r="G150">
+        <v>72.85714285714286</v>
+      </c>
+      <c r="H150">
+        <v>97.82608695652175</v>
+      </c>
     </row>
     <row r="151">
       <c r="B151" t="str">
@@ -2903,6 +3785,12 @@
       <c r="F151">
         <v>9.2</v>
       </c>
+      <c r="G151">
+        <v>24.285714285714285</v>
+      </c>
+      <c r="H151">
+        <v>100</v>
+      </c>
     </row>
     <row r="152">
       <c r="B152" t="str">
@@ -2920,6 +3808,12 @@
       <c r="F152">
         <v>23.3</v>
       </c>
+      <c r="G152">
+        <v>100</v>
+      </c>
+      <c r="H152">
+        <v>100</v>
+      </c>
     </row>
     <row r="153">
       <c r="B153" t="str">
@@ -2937,6 +3831,12 @@
       <c r="F153">
         <v>72.8</v>
       </c>
+      <c r="G153">
+        <v>42.391304347826086</v>
+      </c>
+      <c r="H153">
+        <v>312.44635193133047</v>
+      </c>
     </row>
     <row r="154">
       <c r="B154" t="str">
@@ -2954,6 +3854,12 @@
       <c r="F154">
         <v>12.8</v>
       </c>
+      <c r="G154">
+        <v>14.565217391304348</v>
+      </c>
+      <c r="H154">
+        <v>54.93562231759657</v>
+      </c>
     </row>
     <row r="155">
       <c r="B155" t="str">
@@ -2971,6 +3877,12 @@
       <c r="F155">
         <v>5.4</v>
       </c>
+      <c r="G155">
+        <v>100</v>
+      </c>
+      <c r="H155">
+        <v>100</v>
+      </c>
     </row>
     <row r="156">
       <c r="B156" t="str">
@@ -2988,6 +3900,12 @@
       <c r="F156">
         <v>5</v>
       </c>
+      <c r="G156">
+        <v>84.12698412698413</v>
+      </c>
+      <c r="H156">
+        <v>92.59259259259258</v>
+      </c>
     </row>
     <row r="157">
       <c r="B157" t="str">
@@ -3005,6 +3923,12 @@
       <c r="F157">
         <v>5.5</v>
       </c>
+      <c r="G157">
+        <v>7.936507936507937</v>
+      </c>
+      <c r="H157">
+        <v>101.85185185185185</v>
+      </c>
     </row>
     <row r="158">
       <c r="B158" t="str">
@@ -3022,6 +3946,12 @@
       <c r="F158">
         <v>13.8</v>
       </c>
+      <c r="G158">
+        <v>100</v>
+      </c>
+      <c r="H158">
+        <v>100</v>
+      </c>
     </row>
     <row r="159">
       <c r="B159" t="str">
@@ -3039,6 +3969,12 @@
       <c r="F159">
         <v>16.5</v>
       </c>
+      <c r="G159">
+        <v>8.474576271186441</v>
+      </c>
+      <c r="H159">
+        <v>119.56521739130434</v>
+      </c>
     </row>
     <row r="160">
       <c r="B160" t="str">
@@ -3056,6 +3992,12 @@
       <c r="F160">
         <v>13.1</v>
       </c>
+      <c r="G160">
+        <v>4.745762711864407</v>
+      </c>
+      <c r="H160">
+        <v>94.92753623188405</v>
+      </c>
     </row>
     <row r="161">
       <c r="B161" t="str">
@@ -3073,6 +4015,12 @@
       <c r="F161">
         <v>10.1</v>
       </c>
+      <c r="G161">
+        <v>100</v>
+      </c>
+      <c r="H161">
+        <v>100</v>
+      </c>
     </row>
     <row r="162">
       <c r="B162" t="str">
@@ -3090,6 +4038,12 @@
       <c r="F162">
         <v>10.5</v>
       </c>
+      <c r="G162">
+        <v>48.86363636363637</v>
+      </c>
+      <c r="H162">
+        <v>103.96039603960396</v>
+      </c>
     </row>
     <row r="163">
       <c r="B163" t="str">
@@ -3107,6 +4061,12 @@
       <c r="F163">
         <v>14.1</v>
       </c>
+      <c r="G163">
+        <v>37.5</v>
+      </c>
+      <c r="H163">
+        <v>139.6039603960396</v>
+      </c>
     </row>
     <row r="164">
       <c r="B164" t="str">
@@ -3124,6 +4084,12 @@
       <c r="F164">
         <v>7.7</v>
       </c>
+      <c r="G164">
+        <v>100</v>
+      </c>
+      <c r="H164">
+        <v>100</v>
+      </c>
     </row>
     <row r="165">
       <c r="B165" t="str">
@@ -3141,6 +4107,12 @@
       <c r="F165">
         <v>7.9</v>
       </c>
+      <c r="G165">
+        <v>29.661016949152543</v>
+      </c>
+      <c r="H165">
+        <v>102.59740259740259</v>
+      </c>
     </row>
     <row r="166">
       <c r="B166" t="str">
@@ -3158,6 +4130,12 @@
       <c r="F166">
         <v>6.8</v>
       </c>
+      <c r="G166">
+        <v>17.51412429378531</v>
+      </c>
+      <c r="H166">
+        <v>88.31168831168831</v>
+      </c>
     </row>
     <row r="167">
       <c r="B167" t="str">
@@ -3175,6 +4153,12 @@
       <c r="F167">
         <v>6.8</v>
       </c>
+      <c r="G167">
+        <v>100</v>
+      </c>
+      <c r="H167">
+        <v>100</v>
+      </c>
     </row>
     <row r="168">
       <c r="B168" t="str">
@@ -3192,6 +4176,12 @@
       <c r="F168">
         <v>9.6</v>
       </c>
+      <c r="G168">
+        <v>57.38636363636363</v>
+      </c>
+      <c r="H168">
+        <v>141.1764705882353</v>
+      </c>
     </row>
     <row r="169">
       <c r="B169" t="str">
@@ -3209,6 +4199,12 @@
       <c r="F169">
         <v>9.4</v>
       </c>
+      <c r="G169">
+        <v>14.772727272727273</v>
+      </c>
+      <c r="H169">
+        <v>138.23529411764707</v>
+      </c>
     </row>
     <row r="170">
       <c r="B170" t="str">
@@ -3226,6 +4222,12 @@
       <c r="F170">
         <v>29</v>
       </c>
+      <c r="G170">
+        <v>100</v>
+      </c>
+      <c r="H170">
+        <v>100</v>
+      </c>
     </row>
     <row r="171">
       <c r="B171" t="str">
@@ -3243,6 +4245,12 @@
       <c r="F171">
         <v>24.4</v>
       </c>
+      <c r="G171">
+        <v>61.904761904761905</v>
+      </c>
+      <c r="H171">
+        <v>84.13793103448276</v>
+      </c>
     </row>
     <row r="172">
       <c r="B172" t="str">
@@ -3260,6 +4268,12 @@
       <c r="F172">
         <v>18.7</v>
       </c>
+      <c r="G172">
+        <v>19.841269841269842</v>
+      </c>
+      <c r="H172">
+        <v>64.48275862068965</v>
+      </c>
     </row>
     <row r="173">
       <c r="B173" t="str">
@@ -3277,6 +4291,12 @@
       <c r="F173">
         <v>5.3</v>
       </c>
+      <c r="G173">
+        <v>100</v>
+      </c>
+      <c r="H173">
+        <v>100</v>
+      </c>
     </row>
     <row r="174">
       <c r="B174" t="str">
@@ -3294,6 +4314,12 @@
       <c r="F174">
         <v>8.2</v>
       </c>
+      <c r="G174">
+        <v>31.16883116883117</v>
+      </c>
+      <c r="H174">
+        <v>154.71698113207546</v>
+      </c>
     </row>
     <row r="175">
       <c r="B175" t="str">
@@ -3311,6 +4337,12 @@
       <c r="F175">
         <v>5.5</v>
       </c>
+      <c r="G175">
+        <v>18.181818181818183</v>
+      </c>
+      <c r="H175">
+        <v>103.77358490566039</v>
+      </c>
     </row>
     <row r="176">
       <c r="B176" t="str">
@@ -3328,6 +4360,12 @@
       <c r="F176">
         <v>15</v>
       </c>
+      <c r="G176">
+        <v>100</v>
+      </c>
+      <c r="H176">
+        <v>100</v>
+      </c>
     </row>
     <row r="177">
       <c r="B177" t="str">
@@ -3345,6 +4383,12 @@
       <c r="F177">
         <v>22.3</v>
       </c>
+      <c r="G177">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="H177">
+        <v>148.66666666666666</v>
+      </c>
     </row>
     <row r="178">
       <c r="B178" t="str">
@@ -3362,6 +4406,12 @@
       <c r="F178">
         <v>14.1</v>
       </c>
+      <c r="G178">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="H178">
+        <v>94</v>
+      </c>
     </row>
     <row r="179">
       <c r="B179" t="str">
@@ -3379,6 +4429,12 @@
       <c r="F179">
         <v>13.5</v>
       </c>
+      <c r="G179">
+        <v>100</v>
+      </c>
+      <c r="H179">
+        <v>100</v>
+      </c>
     </row>
     <row r="180">
       <c r="B180" t="str">
@@ -3396,6 +4452,12 @@
       <c r="F180">
         <v>29.4</v>
       </c>
+      <c r="G180">
+        <v>68.35443037974683</v>
+      </c>
+      <c r="H180">
+        <v>217.77777777777777</v>
+      </c>
     </row>
     <row r="181">
       <c r="B181" t="str">
@@ -3413,6 +4475,12 @@
       <c r="F181">
         <v>31.5</v>
       </c>
+      <c r="G181">
+        <v>48.10126582278481</v>
+      </c>
+      <c r="H181">
+        <v>233.33333333333334</v>
+      </c>
     </row>
     <row r="182">
       <c r="B182" t="str">
@@ -3430,6 +4498,12 @@
       <c r="F182">
         <v>10.4</v>
       </c>
+      <c r="G182">
+        <v>100</v>
+      </c>
+      <c r="H182">
+        <v>100</v>
+      </c>
     </row>
     <row r="183">
       <c r="B183" t="str">
@@ -3447,6 +4521,12 @@
       <c r="F183">
         <v>7.8</v>
       </c>
+      <c r="G183">
+        <v>31.914893617021278</v>
+      </c>
+      <c r="H183">
+        <v>75</v>
+      </c>
     </row>
     <row r="184">
       <c r="B184" t="str">
@@ -3464,6 +4544,12 @@
       <c r="F184">
         <v>9.5</v>
       </c>
+      <c r="G184">
+        <v>17.02127659574468</v>
+      </c>
+      <c r="H184">
+        <v>91.34615384615384</v>
+      </c>
     </row>
     <row r="185">
       <c r="B185" t="str">
@@ -3481,6 +4567,12 @@
       <c r="F185">
         <v>27.4</v>
       </c>
+      <c r="G185">
+        <v>100</v>
+      </c>
+      <c r="H185">
+        <v>100</v>
+      </c>
     </row>
     <row r="186">
       <c r="B186" t="str">
@@ -3498,6 +4590,12 @@
       <c r="F186">
         <v>18.2</v>
       </c>
+      <c r="G186">
+        <v>75.625</v>
+      </c>
+      <c r="H186">
+        <v>66.42335766423358</v>
+      </c>
     </row>
     <row r="187">
       <c r="B187" t="str">
@@ -3515,6 +4613,12 @@
       <c r="F187">
         <v>35.5</v>
       </c>
+      <c r="G187">
+        <v>18.75</v>
+      </c>
+      <c r="H187">
+        <v>129.56204379562044</v>
+      </c>
     </row>
     <row r="188">
       <c r="B188" t="str">
@@ -3532,6 +4636,12 @@
       <c r="F188">
         <v>21.1</v>
       </c>
+      <c r="G188">
+        <v>100</v>
+      </c>
+      <c r="H188">
+        <v>100</v>
+      </c>
     </row>
     <row r="189">
       <c r="B189" t="str">
@@ -3549,6 +4659,12 @@
       <c r="F189">
         <v>37.5</v>
       </c>
+      <c r="G189">
+        <v>38.9937106918239</v>
+      </c>
+      <c r="H189">
+        <v>177.7251184834123</v>
+      </c>
     </row>
     <row r="190">
       <c r="B190" t="str">
@@ -3566,6 +4682,12 @@
       <c r="F190">
         <v>18.3</v>
       </c>
+      <c r="G190">
+        <v>30.81761006289308</v>
+      </c>
+      <c r="H190">
+        <v>86.7298578199052</v>
+      </c>
     </row>
     <row r="191">
       <c r="B191" t="str">
@@ -3583,6 +4705,12 @@
       <c r="F191">
         <v>27.9</v>
       </c>
+      <c r="G191">
+        <v>100</v>
+      </c>
+      <c r="H191">
+        <v>100</v>
+      </c>
     </row>
     <row r="192">
       <c r="B192" t="str">
@@ -3600,6 +4728,12 @@
       <c r="F192">
         <v>60.8</v>
       </c>
+      <c r="G192">
+        <v>91.83673469387755</v>
+      </c>
+      <c r="H192">
+        <v>217.92114695340504</v>
+      </c>
     </row>
     <row r="193">
       <c r="B193" t="str">
@@ -3617,6 +4751,12 @@
       <c r="F193">
         <v>39.9</v>
       </c>
+      <c r="G193">
+        <v>55.10204081632653</v>
+      </c>
+      <c r="H193">
+        <v>143.01075268817206</v>
+      </c>
     </row>
     <row r="194">
       <c r="B194" t="str">
@@ -3634,6 +4774,12 @@
       <c r="F194">
         <v>14.9</v>
       </c>
+      <c r="G194">
+        <v>100</v>
+      </c>
+      <c r="H194">
+        <v>100</v>
+      </c>
     </row>
     <row r="195">
       <c r="B195" t="str">
@@ -3651,6 +4797,12 @@
       <c r="F195">
         <v>5</v>
       </c>
+      <c r="G195">
+        <v>80</v>
+      </c>
+      <c r="H195">
+        <v>33.557046979865774</v>
+      </c>
     </row>
     <row r="196">
       <c r="B196" t="str">
@@ -3668,6 +4820,12 @@
       <c r="F196">
         <v>4.6</v>
       </c>
+      <c r="G196">
+        <v>20</v>
+      </c>
+      <c r="H196">
+        <v>30.872483221476507</v>
+      </c>
     </row>
     <row r="197">
       <c r="B197" t="str">
@@ -3685,6 +4843,12 @@
       <c r="F197">
         <v>20.7</v>
       </c>
+      <c r="G197">
+        <v>100</v>
+      </c>
+      <c r="H197">
+        <v>100</v>
+      </c>
     </row>
     <row r="198">
       <c r="B198" t="str">
@@ -3702,6 +4866,12 @@
       <c r="F198">
         <v>13.5</v>
       </c>
+      <c r="G198">
+        <v>50.40650406504065</v>
+      </c>
+      <c r="H198">
+        <v>65.21739130434783</v>
+      </c>
     </row>
     <row r="199">
       <c r="B199" t="str">
@@ -3719,6 +4889,12 @@
       <c r="F199">
         <v>0</v>
       </c>
+      <c r="G199">
+        <v>13.821138211382113</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="B200" t="str">
@@ -3736,6 +4912,12 @@
       <c r="F200">
         <v>31.1</v>
       </c>
+      <c r="G200">
+        <v>100</v>
+      </c>
+      <c r="H200">
+        <v>100</v>
+      </c>
     </row>
     <row r="201">
       <c r="B201" t="str">
@@ -3753,6 +4935,12 @@
       <c r="F201">
         <v>25.8</v>
       </c>
+      <c r="G201">
+        <v>62.5</v>
+      </c>
+      <c r="H201">
+        <v>82.95819935691318</v>
+      </c>
     </row>
     <row r="202">
       <c r="B202" t="str">
@@ -3770,6 +4958,12 @@
       <c r="F202">
         <v>28.2</v>
       </c>
+      <c r="G202">
+        <v>57.5</v>
+      </c>
+      <c r="H202">
+        <v>90.67524115755627</v>
+      </c>
     </row>
     <row r="203">
       <c r="B203" t="str">
@@ -3787,6 +4981,12 @@
       <c r="F203">
         <v>15.8</v>
       </c>
+      <c r="G203">
+        <v>100</v>
+      </c>
+      <c r="H203">
+        <v>100</v>
+      </c>
     </row>
     <row r="204">
       <c r="B204" t="str">
@@ -3804,6 +5004,12 @@
       <c r="F204">
         <v>27.4</v>
       </c>
+      <c r="G204">
+        <v>85.4368932038835</v>
+      </c>
+      <c r="H204">
+        <v>173.41772151898732</v>
+      </c>
     </row>
     <row r="205">
       <c r="B205" t="str">
@@ -3821,6 +5027,12 @@
       <c r="F205">
         <v>8</v>
       </c>
+      <c r="G205">
+        <v>27.184466019417474</v>
+      </c>
+      <c r="H205">
+        <v>50.63291139240506</v>
+      </c>
     </row>
     <row r="206">
       <c r="B206" t="str">
@@ -3838,6 +5050,12 @@
       <c r="F206">
         <v>25.5</v>
       </c>
+      <c r="G206">
+        <v>100</v>
+      </c>
+      <c r="H206">
+        <v>100</v>
+      </c>
     </row>
     <row r="207">
       <c r="B207" t="str">
@@ -3855,6 +5073,12 @@
       <c r="F207">
         <v>23.8</v>
       </c>
+      <c r="G207">
+        <v>81.63265306122449</v>
+      </c>
+      <c r="H207">
+        <v>93.33333333333333</v>
+      </c>
     </row>
     <row r="208">
       <c r="B208" t="str">
@@ -3872,6 +5096,12 @@
       <c r="F208">
         <v>27.4</v>
       </c>
+      <c r="G208">
+        <v>32.6530612244898</v>
+      </c>
+      <c r="H208">
+        <v>107.45098039215686</v>
+      </c>
     </row>
     <row r="209">
       <c r="B209" t="str">
@@ -3889,6 +5119,12 @@
       <c r="F209">
         <v>20.9</v>
       </c>
+      <c r="G209">
+        <v>100</v>
+      </c>
+      <c r="H209">
+        <v>100</v>
+      </c>
     </row>
     <row r="210">
       <c r="B210" t="str">
@@ -3906,6 +5142,12 @@
       <c r="F210">
         <v>26</v>
       </c>
+      <c r="G210">
+        <v>96.875</v>
+      </c>
+      <c r="H210">
+        <v>124.4019138755981</v>
+      </c>
     </row>
     <row r="211">
       <c r="B211" t="str">
@@ -3923,6 +5165,12 @@
       <c r="F211">
         <v>22.5</v>
       </c>
+      <c r="G211">
+        <v>40.625</v>
+      </c>
+      <c r="H211">
+        <v>107.6555023923445</v>
+      </c>
     </row>
     <row r="212">
       <c r="B212" t="str">
@@ -3940,6 +5188,12 @@
       <c r="F212">
         <v>12.7</v>
       </c>
+      <c r="G212">
+        <v>100</v>
+      </c>
+      <c r="H212">
+        <v>100</v>
+      </c>
     </row>
     <row r="213">
       <c r="B213" t="str">
@@ -3957,6 +5211,12 @@
       <c r="F213">
         <v>9.7</v>
       </c>
+      <c r="G213">
+        <v>100</v>
+      </c>
+      <c r="H213">
+        <v>76.37795275590551</v>
+      </c>
     </row>
     <row r="214">
       <c r="B214" t="str">
@@ -3974,6 +5234,12 @@
       <c r="F214">
         <v>8.9</v>
       </c>
+      <c r="G214">
+        <v>34.04255319148936</v>
+      </c>
+      <c r="H214">
+        <v>70.07874015748033</v>
+      </c>
     </row>
     <row r="215">
       <c r="B215" t="str">
@@ -3991,6 +5257,12 @@
       <c r="F215">
         <v>13.2</v>
       </c>
+      <c r="G215">
+        <v>100</v>
+      </c>
+      <c r="H215">
+        <v>100</v>
+      </c>
     </row>
     <row r="216">
       <c r="B216" t="str">
@@ -4008,6 +5280,12 @@
       <c r="F216">
         <v>16.6</v>
       </c>
+      <c r="G216">
+        <v>18.27956989247312</v>
+      </c>
+      <c r="H216">
+        <v>125.75757575757578</v>
+      </c>
     </row>
     <row r="217">
       <c r="B217" t="str">
@@ -4025,6 +5303,12 @@
       <c r="F217">
         <v>0</v>
       </c>
+      <c r="G217">
+        <v>17.204301075268816</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
     </row>
     <row r="218">
       <c r="B218" t="str">
@@ -4042,6 +5326,12 @@
       <c r="F218">
         <v>45.7</v>
       </c>
+      <c r="G218">
+        <v>100</v>
+      </c>
+      <c r="H218">
+        <v>100</v>
+      </c>
     </row>
     <row r="219">
       <c r="B219" t="str">
@@ -4059,6 +5349,12 @@
       <c r="F219">
         <v>54.8</v>
       </c>
+      <c r="G219">
+        <v>43.13725490196079</v>
+      </c>
+      <c r="H219">
+        <v>119.9124726477024</v>
+      </c>
     </row>
     <row r="220">
       <c r="B220" t="str">
@@ -4076,6 +5372,12 @@
       <c r="F220">
         <v>82.3</v>
       </c>
+      <c r="G220">
+        <v>9.803921568627452</v>
+      </c>
+      <c r="H220">
+        <v>180.08752735229757</v>
+      </c>
     </row>
     <row r="221">
       <c r="B221" t="str">
@@ -4093,6 +5395,12 @@
       <c r="F221">
         <v>15.9</v>
       </c>
+      <c r="G221">
+        <v>100</v>
+      </c>
+      <c r="H221">
+        <v>100</v>
+      </c>
     </row>
     <row r="222">
       <c r="B222" t="str">
@@ -4110,6 +5418,12 @@
       <c r="F222">
         <v>12</v>
       </c>
+      <c r="G222">
+        <v>47.82608695652174</v>
+      </c>
+      <c r="H222">
+        <v>75.47169811320755</v>
+      </c>
     </row>
     <row r="223">
       <c r="B223" t="str">
@@ -4127,6 +5441,12 @@
       <c r="F223">
         <v>14.3</v>
       </c>
+      <c r="G223">
+        <v>15.942028985507246</v>
+      </c>
+      <c r="H223">
+        <v>89.937106918239</v>
+      </c>
     </row>
     <row r="224">
       <c r="B224" t="str">
@@ -4144,6 +5464,12 @@
       <c r="F224">
         <v>24.5</v>
       </c>
+      <c r="G224">
+        <v>100</v>
+      </c>
+      <c r="H224">
+        <v>100</v>
+      </c>
     </row>
     <row r="225">
       <c r="B225" t="str">
@@ -4161,6 +5487,12 @@
       <c r="F225">
         <v>37.4</v>
       </c>
+      <c r="G225">
+        <v>42.10526315789474</v>
+      </c>
+      <c r="H225">
+        <v>152.6530612244898</v>
+      </c>
     </row>
     <row r="226">
       <c r="B226" t="str">
@@ -4178,6 +5510,12 @@
       <c r="F226">
         <v>36.3</v>
       </c>
+      <c r="G226">
+        <v>26.31578947368421</v>
+      </c>
+      <c r="H226">
+        <v>148.16326530612244</v>
+      </c>
     </row>
     <row r="227">
       <c r="B227" t="str">
@@ -4195,6 +5533,12 @@
       <c r="F227">
         <v>0</v>
       </c>
+      <c r="G227">
+        <v>100</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="B228" t="str">
@@ -4212,6 +5556,12 @@
       <c r="F228">
         <v>0</v>
       </c>
+      <c r="G228">
+        <v>46.42857142857143</v>
+      </c>
+      <c r="H228">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="B229" t="str">
@@ -4229,6 +5579,12 @@
       <c r="F229">
         <v>0</v>
       </c>
+      <c r="G229">
+        <v>12.5</v>
+      </c>
+      <c r="H229">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="B230" t="str">
@@ -4246,6 +5602,12 @@
       <c r="F230">
         <v>33.3</v>
       </c>
+      <c r="G230">
+        <v>100</v>
+      </c>
+      <c r="H230">
+        <v>100</v>
+      </c>
     </row>
     <row r="231">
       <c r="B231" t="str">
@@ -4263,6 +5625,12 @@
       <c r="F231">
         <v>61</v>
       </c>
+      <c r="G231">
+        <v>37.77777777777778</v>
+      </c>
+      <c r="H231">
+        <v>183.1831831831832</v>
+      </c>
     </row>
     <row r="232">
       <c r="B232" t="str">
@@ -4280,6 +5648,12 @@
       <c r="F232">
         <v>48.8</v>
       </c>
+      <c r="G232">
+        <v>11.11111111111111</v>
+      </c>
+      <c r="H232">
+        <v>146.54654654654655</v>
+      </c>
     </row>
     <row r="233">
       <c r="B233" t="str">
@@ -4297,6 +5671,12 @@
       <c r="F233">
         <v>26.4</v>
       </c>
+      <c r="G233">
+        <v>100</v>
+      </c>
+      <c r="H233">
+        <v>100</v>
+      </c>
     </row>
     <row r="234">
       <c r="B234" t="str">
@@ -4314,6 +5694,12 @@
       <c r="F234">
         <v>17.4</v>
       </c>
+      <c r="G234">
+        <v>26.31578947368421</v>
+      </c>
+      <c r="H234">
+        <v>65.9090909090909</v>
+      </c>
     </row>
     <row r="235">
       <c r="B235" t="str">
@@ -4331,6 +5717,12 @@
       <c r="F235">
         <v>20</v>
       </c>
+      <c r="G235">
+        <v>18.42105263157895</v>
+      </c>
+      <c r="H235">
+        <v>75.75757575757576</v>
+      </c>
     </row>
     <row r="236">
       <c r="B236" t="str">
@@ -4348,6 +5740,12 @@
       <c r="F236">
         <v>37</v>
       </c>
+      <c r="G236">
+        <v>100</v>
+      </c>
+      <c r="H236">
+        <v>100</v>
+      </c>
     </row>
     <row r="237">
       <c r="B237" t="str">
@@ -4365,6 +5763,12 @@
       <c r="F237">
         <v>32.4</v>
       </c>
+      <c r="G237">
+        <v>75</v>
+      </c>
+      <c r="H237">
+        <v>87.56756756756756</v>
+      </c>
     </row>
     <row r="238">
       <c r="B238" t="str">
@@ -4382,6 +5786,12 @@
       <c r="F238">
         <v>36.5</v>
       </c>
+      <c r="G238">
+        <v>62.5</v>
+      </c>
+      <c r="H238">
+        <v>98.64864864864865</v>
+      </c>
     </row>
     <row r="239">
       <c r="B239" t="str">
@@ -4399,6 +5809,12 @@
       <c r="F239">
         <v>12</v>
       </c>
+      <c r="G239">
+        <v>100</v>
+      </c>
+      <c r="H239">
+        <v>100</v>
+      </c>
     </row>
     <row r="240">
       <c r="B240" t="str">
@@ -4416,6 +5832,12 @@
       <c r="F240">
         <v>13</v>
       </c>
+      <c r="G240">
+        <v>45.90163934426229</v>
+      </c>
+      <c r="H240">
+        <v>108.33333333333333</v>
+      </c>
     </row>
     <row r="241">
       <c r="B241" t="str">
@@ -4433,6 +5855,12 @@
       <c r="F241">
         <v>14.7</v>
       </c>
+      <c r="G241">
+        <v>8.19672131147541</v>
+      </c>
+      <c r="H241">
+        <v>122.5</v>
+      </c>
     </row>
     <row r="242">
       <c r="B242" t="str">
@@ -4450,6 +5878,12 @@
       <c r="F242">
         <v>48.1</v>
       </c>
+      <c r="G242">
+        <v>100</v>
+      </c>
+      <c r="H242">
+        <v>100</v>
+      </c>
     </row>
     <row r="243">
       <c r="B243" t="str">
@@ -4467,6 +5901,12 @@
       <c r="F243">
         <v>65.8</v>
       </c>
+      <c r="G243">
+        <v>34.61538461538461</v>
+      </c>
+      <c r="H243">
+        <v>136.7983367983368</v>
+      </c>
     </row>
     <row r="244">
       <c r="B244" t="str">
@@ -4484,11 +5924,17 @@
       <c r="F244">
         <v>38.3</v>
       </c>
+      <c r="G244">
+        <v>21.153846153846153</v>
+      </c>
+      <c r="H244">
+        <v>79.62577962577961</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F244"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H244"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>